<commit_message>
Enhance welcome message analysis by adding screenshot functionality and improving vendor testing logic. Implemented saveScreenshot function to store screenshots on disk, updated TestResult interface to include screenshot data, and modified Excel output to reflect new screenshot paths. Improved parallel processing of vendor tests for better performance.
</commit_message>
<xml_diff>
--- a/welcome-message-analysis.xlsx
+++ b/welcome-message-analysis.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,6 +406,7 @@
     <col min="2" max="2" width="40.83203125" customWidth="1"/>
     <col min="3" max="3" width="80.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -421,123 +422,136 @@
       <c r="D1" t="str">
         <v>Was Detected</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="E1" t="str">
+        <v>Screenshot Path</v>
+      </c>
+    </row>
+    <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Drift</v>
+        <v>Tidio</v>
       </c>
       <c r="B2" t="str">
-        <v>https://www.drift.com/</v>
-      </c>
-      <c r="C2" t="str">
-        <v>No chatbot widget found for analysis.</v>
+        <v>https://www.tidio.com/</v>
+      </c>
+      <c r="C2" t="str" xml:space="preserve">
+        <v xml:space="preserve">The chatbot widget is visible. The welcome message effectively introduces the functionalities by listing clear and relevant options for user assistance. The tone is friendly and inviting, offering help with specific inquiries while also providing a chat option with AI support when the team is offline. 
+Score: 90/100</v>
       </c>
       <c r="D2" t="str">
-        <v>No</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>Yes</v>
+      </c>
+      <c r="E2" t="str">
+        <v>C:\Users\elmun\OneDrive\Escritorio\Zoros\Trabajo\Proyecto OO2\Chatbot-Vendor-Detector\vendor_screenshots\tidio_1743546415881.jpg</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>Intercom</v>
+        <v>LiveChat</v>
       </c>
       <c r="B3" t="str">
-        <v>https://www.intercom.com/</v>
-      </c>
-      <c r="C3" t="str">
-        <v>No chatbot widget found for analysis.</v>
+        <v>https://www.LiveChat.com/</v>
+      </c>
+      <c r="C3" t="str" xml:space="preserve">
+        <v xml:space="preserve">The chatbot widget is visible. The welcome message effectively introduces the main functionality by highlighting engagement tools and invites interaction. 
+Score: 85</v>
       </c>
       <c r="D3" t="str">
         <v>Yes</v>
       </c>
+      <c r="E3" t="str">
+        <v>C:\Users\elmun\OneDrive\Escritorio\Zoros\Trabajo\Proyecto OO2\Chatbot-Vendor-Detector\vendor_screenshots\livechat_1743546440780.jpg</v>
+      </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Tidio</v>
+        <v>HubSpot</v>
       </c>
       <c r="B4" t="str">
-        <v>https://www.tidio.com/</v>
+        <v>https://www.hubspot.com/</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Chatbot widget found for analysis.
-Analyzed Messages:
-1. "Hi there! 👋 Welcome to Tidio Support! We're ready to help you 🥲"
-2. "What is Lyro?"
-3. "Discover Tidio Premium"
-4. "How can I log into my account?"
-5. "How can I manage my subscription?"
-6. "How can I learn about Tidio?"
-Score: 85/100
-The messages effectively introduce the main functionalities and offer easy navigation to common user queries.</v>
+        <v xml:space="preserve">The chatbot widget is visible. 
+The welcome message effectively presents clear options for user engagement, such as "Get free training," "Get started free," "Book a demo," and "Chat with sales." These options introduce the chatbot's functionalities well and guide user interaction effectively.
+Score: 85/100</v>
       </c>
       <c r="D4" t="str">
         <v>Yes</v>
       </c>
+      <c r="E4" t="str">
+        <v>C:\Users\elmun\OneDrive\Escritorio\Zoros\Trabajo\Proyecto OO2\Chatbot-Vendor-Detector\vendor_screenshots\hubspot_1743546472266.jpg</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>LiveChat</v>
+        <v>ChatBot.com</v>
       </c>
       <c r="B5" t="str">
-        <v>https://www.Live  Chat.com/</v>
+        <v>https://www.chatbot.com/</v>
       </c>
       <c r="C5" t="str">
-        <v>net::ERR_NAME_NOT_RESOLVED at https://www.Live  Chat.com/</v>
+        <v>The chatbot widget is visible. The welcome message is friendly and interactive, offering clear navigation options to guide users through different functionalities like building a chatbot, using it, asking questions, or just browsing. The message effectively introduces the chatbot's capabilities. Score: 90/100.</v>
       </c>
       <c r="D5" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="E5" t="str">
+        <v>C:\Users\elmun\OneDrive\Escritorio\Zoros\Trabajo\Proyecto OO2\Chatbot-Vendor-Detector\vendor_screenshots\chatbot.com_1743546495103.jpg</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Trengo</v>
+      </c>
+      <c r="B6" t="str">
+        <v>https://trengo.com/</v>
+      </c>
+      <c r="C6" t="str">
+        <v>No chatbot widget found for analysis.</v>
+      </c>
+      <c r="D6" t="str">
         <v>No</v>
       </c>
-    </row>
-    <row r="6" xml:space="preserve">
-      <c r="A6" t="str">
-        <v>HubSpot</v>
-      </c>
-      <c r="B6" t="str">
-        <v>https://www.hubspot.com/</v>
-      </c>
-      <c r="C6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Here are the analyzed messages from the chatbot widget:
-1. "Get free training"
-2. "Get started free"
-3. "Book a demo"
-4. "Chat with sales"
-Score: 85
-The chatbot effectively introduces its main functionalities and guides users towards various options available right from the start.</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Yes</v>
+      <c r="E6" t="str">
+        <v>C:\Users\elmun\OneDrive\Escritorio\Zoros\Trabajo\Proyecto OO2\Chatbot-Vendor-Detector\vendor_screenshots\trengo_1743546510074.jpg</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Genesys</v>
+        <v>Verloop</v>
       </c>
       <c r="B7" t="str">
-        <v>https://www.genesys.com/</v>
+        <v>https://www.verloop.io/</v>
       </c>
       <c r="C7" t="str">
         <v>No chatbot widget found for analysis.</v>
       </c>
       <c r="D7" t="str">
-        <v>Yes</v>
+        <v>No</v>
+      </c>
+      <c r="E7" t="str">
+        <v>C:\Users\elmun\OneDrive\Escritorio\Zoros\Trabajo\Proyecto OO2\Chatbot-Vendor-Detector\vendor_screenshots\verloop_1743546527205.jpg</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>ChatBot.com</v>
+        <v>kommunicate</v>
       </c>
       <c r="B8" t="str">
-        <v>https://www.chatbot.com/</v>
+        <v>https://www.kommunicate.io/</v>
       </c>
       <c r="C8" t="str">
-        <v>No chatbot widget found for analysis.</v>
+        <v>The chatbot widget is visible, but it doesn't provide any welcome messages introducing functionalities or tutorials. Score: 20.</v>
       </c>
       <c r="D8" t="str">
         <v>Yes</v>
       </c>
+      <c r="E8" t="str">
+        <v>C:\Users\elmun\OneDrive\Escritorio\Zoros\Trabajo\Proyecto OO2\Chatbot-Vendor-Detector\vendor_screenshots\kommunicate_1743546549118.jpg</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>